<commit_message>
corrigindo copiada e colada errada em c4 do 7.6
</commit_message>
<xml_diff>
--- a/doc/ACAP MODELO - Copia.xlsx
+++ b/doc/ACAP MODELO - Copia.xlsx
@@ -18,7 +18,7 @@
   <calcPr calcId="144525"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mg5xRH/pU7zO8Cy6SsiUmRwvCElkA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="" roundtripDataSignature="AMtx7mg5xRH/pU7zO8Cy6SsiUmRwvCElkA=="/>
     </ext>
   </extLst>
 </workbook>
@@ -1046,16 +1046,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FFA8D08D"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1278,11 +1269,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="122312576"/>
-        <c:axId val="122314752"/>
+        <c:axId val="31744768"/>
+        <c:axId val="31746688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122312576"/>
+        <c:axId val="31744768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1328,7 +1319,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122314752"/>
+        <c:crossAx val="31746688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1336,7 +1327,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122314752"/>
+        <c:axId val="31746688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1385,7 +1376,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122312576"/>
+        <c:crossAx val="31744768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1607,11 +1598,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="122559488"/>
-        <c:axId val="122582144"/>
+        <c:axId val="117345664"/>
+        <c:axId val="117351936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122559488"/>
+        <c:axId val="117345664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1631,10 +1622,11 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1656,7 +1648,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122582144"/>
+        <c:crossAx val="117351936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1664,7 +1656,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122582144"/>
+        <c:axId val="117351936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1684,10 +1676,11 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
@@ -1712,7 +1705,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122559488"/>
+        <c:crossAx val="117345664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1902,11 +1895,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="122619392"/>
-        <c:axId val="122621312"/>
+        <c:axId val="121636736"/>
+        <c:axId val="121647104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122619392"/>
+        <c:axId val="121636736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1926,10 +1919,11 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1951,7 +1945,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122621312"/>
+        <c:crossAx val="121647104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1959,7 +1953,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122621312"/>
+        <c:axId val="121647104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1979,10 +1973,11 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
@@ -2007,7 +2002,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122619392"/>
+        <c:crossAx val="121636736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2209,545 +2204,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="122679296"/>
-        <c:axId val="122681216"/>
+        <c:axId val="121684352"/>
+        <c:axId val="121686272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122679296"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr sz="900" b="0" i="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="122681216"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="122681216"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr sz="900" b="0" i="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="122679296"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Dados sem e com ABAP'!$B$2:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:trendline>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:val>
-            <c:numRef>
-              <c:f>'Dados sem e com ABAP'!$C$2:$C$9</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>177870</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>682463.66666666674</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1920088.3333333335</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3700044</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5678735</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7775134.666666666</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10274399</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12822530</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:trendline>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:val>
-            <c:numRef>
-              <c:f>'Dados sem e com ABAP'!$D$2:$D$9</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>488564.33333333326</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9549013.6666666679</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>36625191.333333328</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>82587247.666666672</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>144689629</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>210361262.33333334</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>275669970.33333337</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>335806819.33333331</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="91848064"/>
-        <c:axId val="91870336"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="91848064"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91870336"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="91870336"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91848064"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
-  <c:roundedCorners val="1"/>
-  <c:style val="2"/>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cmpd="sng">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Dados sem e com ABAP'!$B$10:$B$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Dados sem e com ABAP'!$C$10:$C$17</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>257385.66666666674</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2624265.666666667</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8369270.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13120080</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>19132261</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>23366941</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>27383958.333333332</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>30942047</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="28575" cmpd="sng">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Dados sem e com ABAP'!$B$10:$B$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Dados sem e com ABAP'!$D$10:$D$17</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>997800.33333333326</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16921914.333333332</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>62446266</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>127644898.33333333</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>204813255.66666666</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>283987235.66666669</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>356881453</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>417939598</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="122344192"/>
-        <c:axId val="122346112"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="122344192"/>
+        <c:axId val="121684352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2793,7 +2254,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122346112"/>
+        <c:crossAx val="121686272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2801,7 +2262,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122346112"/>
+        <c:axId val="121686272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2850,7 +2311,316 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122344192"/>
+        <c:crossAx val="121684352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Dados sem e com ABAP'!$B$10:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Dados sem e com ABAP'!$C$10:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>257385.66666666674</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2624265.666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8369270.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13120080</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19132261</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23366941</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27383958.333333332</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30942047</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Dados sem e com ABAP'!$B$10:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Dados sem e com ABAP'!$D$10:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>997800.33333333326</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16921914.333333332</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62446266</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>127644898.33333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>204813255.66666666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>283987235.66666669</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>356881453</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>417939598</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="31759744"/>
+        <c:axId val="31774208"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="31759744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="900" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="31774208"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="31774208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="900" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="31759744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3052,11 +2822,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="122374016"/>
-        <c:axId val="122380288"/>
+        <c:axId val="31340416"/>
+        <c:axId val="31346688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122374016"/>
+        <c:axId val="31340416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3102,7 +2872,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122380288"/>
+        <c:crossAx val="31346688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3110,7 +2880,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122380288"/>
+        <c:axId val="31346688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3159,7 +2929,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122374016"/>
+        <c:crossAx val="31340416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3361,11 +3131,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="122392576"/>
-        <c:axId val="122394496"/>
+        <c:axId val="31355264"/>
+        <c:axId val="31357184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122392576"/>
+        <c:axId val="31355264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3411,7 +3181,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122394496"/>
+        <c:crossAx val="31357184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3419,7 +3189,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122394496"/>
+        <c:axId val="31357184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3468,7 +3238,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122392576"/>
+        <c:crossAx val="31355264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3670,11 +3440,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="122427648"/>
-        <c:axId val="122429824"/>
+        <c:axId val="93010560"/>
+        <c:axId val="93012736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122427648"/>
+        <c:axId val="93010560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3720,7 +3490,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122429824"/>
+        <c:crossAx val="93012736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3728,7 +3498,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122429824"/>
+        <c:axId val="93012736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3777,7 +3547,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122427648"/>
+        <c:crossAx val="93010560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3988,11 +3758,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="122450688"/>
-        <c:axId val="122452608"/>
+        <c:axId val="93033600"/>
+        <c:axId val="93035520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122450688"/>
+        <c:axId val="93033600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4038,7 +3808,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122452608"/>
+        <c:crossAx val="93035520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4046,7 +3816,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122452608"/>
+        <c:axId val="93035520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4095,7 +3865,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122450688"/>
+        <c:crossAx val="93033600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4297,11 +4067,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="122469376"/>
-        <c:axId val="122492032"/>
+        <c:axId val="93056384"/>
+        <c:axId val="106894848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122469376"/>
+        <c:axId val="93056384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4347,7 +4117,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122492032"/>
+        <c:crossAx val="106894848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4355,7 +4125,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122492032"/>
+        <c:axId val="106894848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4404,7 +4174,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122469376"/>
+        <c:crossAx val="93056384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4620,11 +4390,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="122509568"/>
-        <c:axId val="122511744"/>
+        <c:axId val="106916480"/>
+        <c:axId val="106930944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122509568"/>
+        <c:axId val="106916480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4644,10 +4414,11 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4669,7 +4440,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122511744"/>
+        <c:crossAx val="106930944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4677,7 +4448,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122511744"/>
+        <c:axId val="106930944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4697,10 +4468,11 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
@@ -4725,7 +4497,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122509568"/>
+        <c:crossAx val="106916480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4927,11 +4699,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="122532608"/>
-        <c:axId val="122534528"/>
+        <c:axId val="117331072"/>
+        <c:axId val="117332992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122532608"/>
+        <c:axId val="117331072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4951,10 +4723,11 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4976,7 +4749,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122534528"/>
+        <c:crossAx val="117332992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4984,7 +4757,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122534528"/>
+        <c:axId val="117332992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5004,10 +4777,11 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
@@ -5032,7 +4806,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122532608"/>
+        <c:crossAx val="117331072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5351,36 +5125,6 @@
     </xdr:graphicFrame>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -21585,8 +21329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>